<commit_message>
working on excel filter
</commit_message>
<xml_diff>
--- a/src/configfiles/Valid_Object_Models_and_Types.xlsx
+++ b/src/configfiles/Valid_Object_Models_and_Types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\d2e\src\configfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396CA68B-A49C-4232-88DB-6028F29087C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286DBDF3-89C6-4931-8B7D-37B0923E1D20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8235" yWindow="9345" windowWidth="38700" windowHeight="12405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="57">
   <si>
     <t>GMS_desigo_px_EOT_BA_PX_AI_10</t>
   </si>
@@ -192,13 +192,28 @@
   </si>
   <si>
     <t>Data Type</t>
+  </si>
+  <si>
+    <t>Read Property</t>
+  </si>
+  <si>
+    <t>Present_Value</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>reachable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +230,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,16 +259,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Komma 2" xfId="4" xr:uid="{9D477175-F5CD-43FD-B920-8AA6BB001098}"/>
+    <cellStyle name="Prozent 2" xfId="3" xr:uid="{10B62129-49FE-45E0-8418-03FA576E97E4}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{8F7E644B-96EB-4CBC-80B3-1DAAC15F7E16}"/>
+    <cellStyle name="Standard 3" xfId="5" xr:uid="{C1C1DDB8-0605-4A5B-BE3B-DF7CA5209103}"/>
+    <cellStyle name="Standard 4" xfId="2" xr:uid="{892C2076-B96E-4606-8A39-43468615E4B7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -524,400 +555,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.5703125" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes on objectmodel summary
</commit_message>
<xml_diff>
--- a/src/configfiles/Valid_Object_Models_and_Types.xlsx
+++ b/src/configfiles/Valid_Object_Models_and_Types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20343"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\d2e\src\configfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286DBDF3-89C6-4931-8B7D-37B0923E1D20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664AEFE-29A8-4E20-A60E-DB79BE9B42DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="1020" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="106">
   <si>
     <t>GMS_desigo_px_EOT_BA_PX_AI_10</t>
   </si>
@@ -204,6 +196,153 @@
   </si>
   <si>
     <t>reachable</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_AirFlTck11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_CcgChw11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_CclChw11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_FanOp11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_FanVarSpd11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_FcuTRCtlC11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_FcuTRCtlH11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_FcuVntCtl11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_FpbTCasCtlC11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_FpbTRCtlH11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_HCcg4Pipe11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_HCcg4Pipe13_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_HcgHw11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_HclHw11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_HCStaDtr11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_HvacPltMod11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_HvacPltMod12_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_HvacPltMod13_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_RadHw11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_RHvacCoo11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_RHvacCoo12_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_RHvacCoo13_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_ROpMod11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_ROpUn11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_RpdVntOp11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_SpTR11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_VavEx11_10</t>
+  </si>
+  <si>
+    <t>GMS_s1_room_ctl_EOT_BA_RDS1_APPL_VavSu11_10</t>
+  </si>
+  <si>
+    <t>SpFan1Spd_Present_Value</t>
+  </si>
+  <si>
+    <t>CclVlvPos_Present_Value</t>
+  </si>
+  <si>
+    <t>RcgVlvPosCVal_Present_Value</t>
+  </si>
+  <si>
+    <t>AirFlSuR_Present_Value</t>
+  </si>
+  <si>
+    <t>FanVarSpd_Present_Value</t>
+  </si>
+  <si>
+    <t>PrSpC_Present_Value</t>
+  </si>
+  <si>
+    <t>PrSpH_Present_Value</t>
+  </si>
+  <si>
+    <t>PrSpVnt_Present_Value</t>
+  </si>
+  <si>
+    <t>RcgVlvPosVal_Present_Value</t>
+  </si>
+  <si>
+    <t>RcgVlvPosHVal_Present_Value</t>
+  </si>
+  <si>
+    <t>HclVlvPos_Present_Value</t>
+  </si>
+  <si>
+    <t>HCSta_Present_Value</t>
+  </si>
+  <si>
+    <t>PltOpMod_Present_Value</t>
+  </si>
+  <si>
+    <t>RadVlvPosVal_Present_Value</t>
+  </si>
+  <si>
+    <t>RTemp_Present_Value</t>
+  </si>
+  <si>
+    <t>ROpMod_Present_Value</t>
+  </si>
+  <si>
+    <t>ROpUnCtl_Ds1_Group_Category_Text</t>
+  </si>
+  <si>
+    <t>RpdVnt_Present_Value</t>
+  </si>
+  <si>
+    <t>SpTR_Present_Value</t>
+  </si>
+  <si>
+    <t>VavExSpAirFl_Present_Value</t>
+  </si>
+  <si>
+    <t>VavSuSpAirFl_Present_Value</t>
   </si>
 </sst>
 </file>
@@ -211,7 +350,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -264,7 +403,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
@@ -273,13 +412,24 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Komma 2" xfId="4" xr:uid="{9D477175-F5CD-43FD-B920-8AA6BB001098}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Prozent 2" xfId="3" xr:uid="{10B62129-49FE-45E0-8418-03FA576E97E4}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{8F7E644B-96EB-4CBC-80B3-1DAAC15F7E16}"/>
     <cellStyle name="Standard 3" xfId="5" xr:uid="{C1C1DDB8-0605-4A5B-BE3B-DF7CA5209103}"/>
     <cellStyle name="Standard 4" xfId="2" xr:uid="{892C2076-B96E-4606-8A39-43468615E4B7}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -555,15 +705,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.5703125" customWidth="1"/>
+    <col min="1" max="1" width="63.5703125" customWidth="1"/>
     <col min="2" max="2" width="43.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
@@ -1097,6 +1247,314 @@
         <v>55</v>
       </c>
     </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>69</v>
+      </c>
+      <c r="B61" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" t="s">
+        <v>51</v>
+      </c>
+      <c r="C63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" t="s">
+        <v>48</v>
+      </c>
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" t="s">
+        <v>48</v>
+      </c>
+      <c r="C69" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>83</v>
+      </c>
+      <c r="B75" t="s">
+        <v>48</v>
+      </c>
+      <c r="C75" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C76" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>